<commit_message>
atualizado status e backlog
</commit_message>
<xml_diff>
--- a/Documentação/Product Backlog v1.xlsx
+++ b/Documentação/Product Backlog v1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vinicius\Bandtec\Smart Tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/849c3e71a5d7c7de/Área de Trabalho/Smart Tools/SmartTools-2.0/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E542606F-DEE2-4613-9FAE-405DA3F8DFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{E542606F-DEE2-4613-9FAE-405DA3F8DFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B15316F3-1E73-4916-8332-5E635A81BD7F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -273,49 +273,49 @@
     <t>Deverá ter uma tela onde será mostrado o gráfico com receitas e despesas da oficina. Deverá ter um descritivo com as quantidades e os valores de cada parte do gráfico</t>
   </si>
   <si>
-    <t>Oficina - Dashboard Gráfico</t>
-  </si>
-  <si>
-    <t>Oficina - Dashboard Mais Detalhes</t>
-  </si>
-  <si>
     <t>Deverá existir um botão onde ao clicar levará o usuário a tela de extrato.</t>
   </si>
   <si>
-    <t>Oficina - Extrato</t>
-  </si>
-  <si>
     <t>Sistema deverá ter uma tela de extrato onde o cliente visualizará todas as transações cadastradas.</t>
   </si>
   <si>
-    <t>Oficina - Filtro</t>
-  </si>
-  <si>
     <t>Sistema deverá ter uma opção de filtro, onde poderá filtrar por data definida.</t>
   </si>
   <si>
-    <t>Oficina - Cadastro Cliente</t>
-  </si>
-  <si>
     <t>Sistema deverá ter uma tela com a lista de clientes cadastradas na aplicação.</t>
   </si>
   <si>
-    <t>Oficina - Telas Detalhe</t>
-  </si>
-  <si>
     <t>Sistema deverá ter uma tela onde será detalhado o extrato, cliente e veícúlo com as informações salvas no banco de dados.</t>
   </si>
   <si>
-    <t>Oficina - Botão Nova Aplicação</t>
-  </si>
-  <si>
-    <t>Oficina - Tela Aplicação</t>
-  </si>
-  <si>
     <t>Deverá existir um botão nas telas da dashboard, cliente, extrato onde levará para tela de novas aplicações.</t>
   </si>
   <si>
     <t>Deverá ter uma tela aonde o usuário deverá selecionar qual nova aplicação ele quer cadastrar.</t>
+  </si>
+  <si>
+    <t>Serviços - Extrato</t>
+  </si>
+  <si>
+    <t>Serviços - Telas Detalhe</t>
+  </si>
+  <si>
+    <t>Serviços - Filtro</t>
+  </si>
+  <si>
+    <t>Serviços - Cadastro Cliente</t>
+  </si>
+  <si>
+    <t>Serviços - Botão Nova Aplicação</t>
+  </si>
+  <si>
+    <t>Serviços - Tela Aplicação</t>
+  </si>
+  <si>
+    <t>Serviços - Dashboard Mais Detalhes</t>
+  </si>
+  <si>
+    <t>Serviços - Dashboard Gráfico</t>
   </si>
 </sst>
 </file>
@@ -1916,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:H28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="23.1" customHeight="1"/>
@@ -2060,7 +2060,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="D9" s="30" t="s">
         <v>59</v>
@@ -2077,10 +2077,10 @@
         <v>20</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E10" s="26"/>
       <c r="F10" s="24" t="s">
@@ -2094,10 +2094,10 @@
         <v>20</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E11" s="26"/>
       <c r="F11" s="24"/>
@@ -2111,10 +2111,10 @@
         <v>20</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E12" s="26"/>
       <c r="F12" s="24"/>
@@ -2128,10 +2128,10 @@
         <v>20</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E13" s="26"/>
       <c r="F13" s="24"/>
@@ -2145,10 +2145,10 @@
         <v>20</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E14" s="26"/>
       <c r="F14" s="24"/>
@@ -2165,7 +2165,7 @@
         <v>71</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E15" s="26"/>
       <c r="F15" s="24"/>
@@ -2182,7 +2182,7 @@
         <v>72</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E16" s="26"/>
       <c r="F16" s="24"/>

</xml_diff>